<commit_message>
:globe_with_meridians: :bug: fix typo "Reperaturen" -> "Reparaturen"
Issue abas-specificationsconfigurator-web#76
</commit_message>
<xml_diff>
--- a/resources/excel/de/specification_configurator_template.xlsx
+++ b/resources/excel/de/specification_configurator_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hagen.pommer/Repositories/abas-specificationsconfigurator/api/resources/excel/de/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF19B0F-7A2E-8345-939E-74CB716E7393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0666EA0-58EE-7449-A425-DF8A6AACA33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="67200" windowHeight="35860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="67200" windowHeight="35860" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Firmenprofil" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,9 @@
     <sheet name="7. Projekt" sheetId="7" r:id="rId7"/>
     <sheet name="8. Angaben Softwareanbieter" sheetId="8" r:id="rId8"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2. Organisation'!$A$1:$C$75</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -813,9 +816,6 @@
     <t>Regelmäßige Dienstleistungen und Wartungen</t>
   </si>
   <si>
-    <t>Reperaturen</t>
-  </si>
-  <si>
     <t>Weitere funktionale Anforderungen im Bereich Service:</t>
   </si>
   <si>
@@ -1692,6 +1692,9 @@
   </si>
   <si>
     <t>Anzahl Einkaufsteile (1 bis &gt; 1000)</t>
+  </si>
+  <si>
+    <t>Reparaturen</t>
   </si>
 </sst>
 </file>
@@ -2615,7 +2618,7 @@
     </row>
     <row r="13" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="77" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C13" s="77"/>
     </row>
@@ -2675,7 +2678,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -2711,14 +2714,14 @@
         <v>32</v>
       </c>
       <c r="B26" s="45" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C26" s="45"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="44"/>
       <c r="B27" s="44" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C27" s="44"/>
     </row>
@@ -2734,7 +2737,7 @@
         <v>33</v>
       </c>
       <c r="B29" s="45" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C29" s="45"/>
     </row>
@@ -2757,7 +2760,7 @@
         <v>34</v>
       </c>
       <c r="B32" s="45" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C32" s="45"/>
     </row>
@@ -2810,7 +2813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF85E35C-3C2B-405B-A435-8237A8C583D7}">
   <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="94" zoomScaleNormal="100" zoomScalePageLayoutView="94" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScale="94" zoomScaleNormal="100" zoomScalePageLayoutView="94" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
@@ -2853,7 +2856,7 @@
         <v>98</v>
       </c>
       <c r="C4" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2861,7 +2864,7 @@
         <v>99</v>
       </c>
       <c r="C5" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2869,7 +2872,7 @@
         <v>100</v>
       </c>
       <c r="C6" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2877,7 +2880,7 @@
         <v>101</v>
       </c>
       <c r="C7" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2885,7 +2888,7 @@
         <v>102</v>
       </c>
       <c r="C8" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2893,7 +2896,7 @@
         <v>103</v>
       </c>
       <c r="C9" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2901,7 +2904,7 @@
         <v>104</v>
       </c>
       <c r="C10" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2909,7 +2912,7 @@
         <v>106</v>
       </c>
       <c r="C11" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2917,7 +2920,7 @@
         <v>105</v>
       </c>
       <c r="C12" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2925,7 +2928,7 @@
         <v>107</v>
       </c>
       <c r="C13" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2942,7 +2945,7 @@
         <v>79</v>
       </c>
       <c r="C15" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2950,7 +2953,7 @@
         <v>80</v>
       </c>
       <c r="C16" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2958,15 +2961,15 @@
         <v>81</v>
       </c>
       <c r="C17" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="51" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C18" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2974,7 +2977,7 @@
         <v>82</v>
       </c>
       <c r="C19" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2982,7 +2985,7 @@
         <v>83</v>
       </c>
       <c r="C20" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2990,7 +2993,7 @@
         <v>84</v>
       </c>
       <c r="C21" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2998,7 +3001,7 @@
         <v>92</v>
       </c>
       <c r="C22" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3006,7 +3009,7 @@
         <v>93</v>
       </c>
       <c r="C23" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3014,7 +3017,7 @@
         <v>85</v>
       </c>
       <c r="C24" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3022,7 +3025,7 @@
         <v>86</v>
       </c>
       <c r="C25" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3071,20 +3074,20 @@
     </row>
     <row r="34" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="B34" s="48" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="59.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="48" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B36" s="51" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C36" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="45" x14ac:dyDescent="0.2">
@@ -3094,17 +3097,17 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B38" s="51" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B39" s="51" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B40" s="51" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -3138,7 +3141,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B46" s="51" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -3151,7 +3154,7 @@
         <v>70</v>
       </c>
       <c r="C48" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -3159,7 +3162,7 @@
         <v>71</v>
       </c>
       <c r="C49" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -3167,7 +3170,7 @@
         <v>72</v>
       </c>
       <c r="C50" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -3181,10 +3184,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B52" s="51" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C52" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -3192,7 +3195,7 @@
         <v>62</v>
       </c>
       <c r="C53" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -3200,7 +3203,7 @@
         <v>63</v>
       </c>
       <c r="C54" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -3208,7 +3211,7 @@
         <v>64</v>
       </c>
       <c r="C55" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -3216,7 +3219,7 @@
         <v>65</v>
       </c>
       <c r="C56" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -3224,7 +3227,7 @@
         <v>66</v>
       </c>
       <c r="C57" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -3241,7 +3244,7 @@
         <v>54</v>
       </c>
       <c r="C59" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -3249,7 +3252,7 @@
         <v>55</v>
       </c>
       <c r="C60" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -3257,7 +3260,7 @@
         <v>56</v>
       </c>
       <c r="C61" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -3265,7 +3268,7 @@
         <v>57</v>
       </c>
       <c r="C62" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -3273,7 +3276,7 @@
         <v>58</v>
       </c>
       <c r="C63" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -3281,7 +3284,7 @@
         <v>59</v>
       </c>
       <c r="C64" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -3289,7 +3292,7 @@
         <v>51</v>
       </c>
       <c r="C65" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -3306,7 +3309,7 @@
         <v>50</v>
       </c>
       <c r="C67" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -3314,7 +3317,7 @@
         <v>49</v>
       </c>
       <c r="C68" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -3327,7 +3330,7 @@
         <v>47</v>
       </c>
       <c r="C70" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -3335,7 +3338,7 @@
         <v>46</v>
       </c>
       <c r="C71" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -3352,7 +3355,7 @@
         <v>43</v>
       </c>
       <c r="C73" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -3360,7 +3363,7 @@
         <v>44</v>
       </c>
       <c r="C74" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -3368,7 +3371,7 @@
         <v>45</v>
       </c>
       <c r="C75" s="55" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
   </sheetData>
@@ -3417,7 +3420,7 @@
         <v>109</v>
       </c>
       <c r="B1" s="65" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C1" s="65" t="s">
         <v>114</v>
@@ -3519,7 +3522,7 @@
         <v>125</v>
       </c>
       <c r="C17" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
@@ -3532,7 +3535,7 @@
         <v>131</v>
       </c>
       <c r="C19" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
@@ -3545,7 +3548,7 @@
         <v>132</v>
       </c>
       <c r="C21" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
@@ -3558,7 +3561,7 @@
         <v>133</v>
       </c>
       <c r="C23" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.2">
@@ -3603,10 +3606,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="62" t="s">
+        <v>404</v>
+      </c>
+      <c r="B1" s="63" t="s">
         <v>405</v>
-      </c>
-      <c r="B1" s="63" t="s">
-        <v>406</v>
       </c>
       <c r="C1" s="63" t="s">
         <v>114</v>
@@ -3614,92 +3617,92 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="44" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="B3" s="45" t="s">
         <v>408</v>
-      </c>
-      <c r="B3" s="45" t="s">
-        <v>409</v>
       </c>
       <c r="C3" s="45"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B8" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="B9" s="45" t="s">
         <v>415</v>
-      </c>
-      <c r="B9" s="45" t="s">
-        <v>416</v>
       </c>
       <c r="C9" s="45"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B11" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B12" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B13" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B14" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B15" s="45" t="s">
         <v>233</v>
@@ -3708,438 +3711,438 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B16" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B17" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C17" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B18" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B19" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B20" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C20" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B21" s="45" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C21" s="45"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B22" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B23" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C23" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B24" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B25" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B26" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C26" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
+        <v>418</v>
+      </c>
+      <c r="B27" s="45" t="s">
         <v>419</v>
-      </c>
-      <c r="B27" s="45" t="s">
-        <v>420</v>
       </c>
       <c r="C27" s="45"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B28" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B29" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C29" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B30" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B31" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B32" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C32" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="B33" s="45" t="s">
         <v>421</v>
-      </c>
-      <c r="B33" s="45" t="s">
-        <v>422</v>
       </c>
       <c r="C33" s="45"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B34" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B35" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C35" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B36" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B37" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B38" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C38" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
+        <v>422</v>
+      </c>
+      <c r="B39" s="45" t="s">
         <v>423</v>
-      </c>
-      <c r="B39" s="45" t="s">
-        <v>424</v>
       </c>
       <c r="C39" s="45"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B40" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B41" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C41" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B42" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B43" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B44" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C44" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="B45" s="45" t="s">
         <v>425</v>
-      </c>
-      <c r="B45" s="45" t="s">
-        <v>426</v>
       </c>
       <c r="C45" s="45"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B46" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B47" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C47" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B48" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B49" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B50" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C50" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="B51" s="45" t="s">
         <v>427</v>
-      </c>
-      <c r="B51" s="45" t="s">
-        <v>428</v>
       </c>
       <c r="C51" s="45"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B52" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B53" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C53" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B54" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B55" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B56" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C56" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="B57" s="45" t="s">
         <v>429</v>
-      </c>
-      <c r="B57" s="45" t="s">
-        <v>430</v>
       </c>
       <c r="C57" s="45"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B58" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B59" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C59" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B60" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B61" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B62" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C62" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="B63" s="45" t="s">
         <v>431</v>
-      </c>
-      <c r="B63" s="45" t="s">
-        <v>432</v>
       </c>
       <c r="C63" s="45"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B64" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B65" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C65" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B66" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B67" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B68" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C68" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="B69" s="45" t="s">
         <v>433</v>
-      </c>
-      <c r="B69" s="45" t="s">
-        <v>434</v>
       </c>
       <c r="C69" s="45"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B70" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B71" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C71" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B72" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B73" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B74" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C74" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="B75" s="45" t="s">
         <v>435</v>
-      </c>
-      <c r="B75" s="45" t="s">
-        <v>436</v>
       </c>
       <c r="C75" s="45"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B76" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B77" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C77" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B78" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B79" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B80" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C80" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="8" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B81" s="45" t="s">
         <v>199</v>
@@ -4148,118 +4151,118 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B82" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B83" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C83" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B84" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B85" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B86" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C86" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="B87" s="45" t="s">
         <v>438</v>
-      </c>
-      <c r="B87" s="45" t="s">
-        <v>439</v>
       </c>
       <c r="C87" s="45"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B88" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B89" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C89" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B90" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B91" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B92" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C92" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="B93" s="45" t="s">
         <v>440</v>
-      </c>
-      <c r="B93" s="45" t="s">
-        <v>441</v>
       </c>
       <c r="C93" s="45"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B94" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B95" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C95" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B96" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B97" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B98" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C98" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="8" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B99" s="45" t="s">
         <v>210</v>
@@ -4268,198 +4271,198 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B100" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B101" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C101" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B102" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B103" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B104" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C104" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="8" t="s">
+        <v>442</v>
+      </c>
+      <c r="B105" s="45" t="s">
         <v>443</v>
-      </c>
-      <c r="B105" s="45" t="s">
-        <v>444</v>
       </c>
       <c r="C105" s="45"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B106" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B107" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C107" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B108" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B109" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B110" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C110" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="B111" s="45" t="s">
         <v>445</v>
-      </c>
-      <c r="B111" s="45" t="s">
-        <v>446</v>
       </c>
       <c r="C111" s="45"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B112" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B113" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C113" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B114" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B115" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B116" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C116" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="8" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B117" s="45" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C117" s="45"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B118" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B119" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C119" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B120" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B121" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B122" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C122" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="8" t="s">
+        <v>448</v>
+      </c>
+      <c r="B123" s="45" t="s">
         <v>449</v>
-      </c>
-      <c r="B123" s="45" t="s">
-        <v>450</v>
       </c>
       <c r="C123" s="45"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B124" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B125" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C125" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B126" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B127" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B128" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C128" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="8" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B129" s="45" t="s">
         <v>71</v>
@@ -4468,727 +4471,727 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B130" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B131" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C131" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B132" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B133" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B134" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C134" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="B135" s="45" t="s">
         <v>452</v>
-      </c>
-      <c r="B135" s="45" t="s">
-        <v>453</v>
       </c>
       <c r="C135" s="45"/>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B136" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B137" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C137" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B138" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B139" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B140" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C140" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="8" t="s">
+        <v>453</v>
+      </c>
+      <c r="B141" s="45" t="s">
         <v>454</v>
-      </c>
-      <c r="B141" s="45" t="s">
-        <v>455</v>
       </c>
       <c r="C141" s="45"/>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B142" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B143" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C143" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B144" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B145" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B146" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C146" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="8" t="s">
+        <v>455</v>
+      </c>
+      <c r="B147" s="45" t="s">
         <v>456</v>
-      </c>
-      <c r="B147" s="45" t="s">
-        <v>457</v>
       </c>
       <c r="C147" s="45"/>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B148" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B149" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C149" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B150" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B151" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B152" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C152" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="8" t="s">
+        <v>457</v>
+      </c>
+      <c r="B153" s="45" t="s">
         <v>458</v>
-      </c>
-      <c r="B153" s="45" t="s">
-        <v>459</v>
       </c>
       <c r="C153" s="45"/>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B154" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B155" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C155" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B156" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B157" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B158" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C158" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" s="8" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B159" s="45" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C159" s="45"/>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B160" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B161" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C161" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B162" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B163" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B164" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C164" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" s="8" t="s">
+        <v>460</v>
+      </c>
+      <c r="B165" s="45" t="s">
         <v>461</v>
-      </c>
-      <c r="B165" s="45" t="s">
-        <v>462</v>
       </c>
       <c r="C165" s="45"/>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B166" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B167" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C167" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B168" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B169" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B170" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C170" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" s="8" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B171" s="45" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C171" s="45"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B172" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B173" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C173" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B174" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B175" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B176" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C176" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" s="8" t="s">
+        <v>463</v>
+      </c>
+      <c r="B177" s="45" t="s">
         <v>464</v>
-      </c>
-      <c r="B177" s="45" t="s">
-        <v>465</v>
       </c>
       <c r="C177" s="45"/>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B178" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B179" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C179" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B180" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B181" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B182" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C182" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="B183" s="45" t="s">
         <v>466</v>
-      </c>
-      <c r="B183" s="45" t="s">
-        <v>467</v>
       </c>
       <c r="C183" s="45"/>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B184" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B185" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C185" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B186" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B187" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B188" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C188" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="B189" s="45" t="s">
         <v>468</v>
-      </c>
-      <c r="B189" s="45" t="s">
-        <v>469</v>
       </c>
       <c r="C189" s="45"/>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B190" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B191" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C191" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B192" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B193" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B194" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C194" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" s="8" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B195" s="45" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C195" s="45"/>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B196" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B197" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C197" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B198" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B199" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B200" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C200" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="B201" s="45" t="s">
         <v>471</v>
-      </c>
-      <c r="B201" s="45" t="s">
-        <v>472</v>
       </c>
       <c r="C201" s="45"/>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B202" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B203" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C203" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B204" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B205" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B206" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C206" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="207" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A207" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="B207" s="61" t="s">
         <v>473</v>
-      </c>
-      <c r="B207" s="61" t="s">
-        <v>474</v>
       </c>
       <c r="C207" s="45"/>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B208" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B209" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C209" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B210" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B211" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B212" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C212" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="B213" s="45" t="s">
         <v>475</v>
-      </c>
-      <c r="B213" s="45" t="s">
-        <v>476</v>
       </c>
       <c r="C213" s="45"/>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B214" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B215" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C215" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B216" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B217" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B218" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C218" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A219" s="8" t="s">
+        <v>476</v>
+      </c>
+      <c r="B219" s="45" t="s">
         <v>477</v>
-      </c>
-      <c r="B219" s="45" t="s">
-        <v>478</v>
       </c>
       <c r="C219" s="45"/>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B220" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B221" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C221" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B222" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B223" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B224" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C224" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="B225" s="45" t="s">
         <v>479</v>
-      </c>
-      <c r="B225" s="45" t="s">
-        <v>480</v>
       </c>
       <c r="C225" s="45"/>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B226" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B227" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C227" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B228" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B229" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B230" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C230" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231" s="8" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B231" s="45" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C231" s="45"/>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B232" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B233" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C233" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B234" s="44" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B235" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B236" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C236" s="42" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A237" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="B237" s="45" t="s">
         <v>482</v>
-      </c>
-      <c r="B237" s="45" t="s">
-        <v>483</v>
       </c>
       <c r="C237" s="45"/>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B238" s="44" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>
@@ -5233,7 +5236,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>114</v>
@@ -5246,7 +5249,7 @@
     </row>
     <row r="3" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="74" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>135</v>
@@ -5258,7 +5261,7 @@
         <v>136</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -5266,7 +5269,7 @@
         <v>137</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -5274,7 +5277,7 @@
         <v>138</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -5282,7 +5285,7 @@
         <v>139</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -5290,7 +5293,7 @@
         <v>140</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -5298,12 +5301,12 @@
         <v>141</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="74" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>142</v>
@@ -5315,7 +5318,7 @@
         <v>143</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.2">
@@ -5323,7 +5326,7 @@
         <v>144</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -5331,15 +5334,15 @@
         <v>145</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="74" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C14" s="9"/>
     </row>
@@ -5348,23 +5351,23 @@
         <v>146</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C16" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C17" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.2">
@@ -5372,12 +5375,12 @@
         <v>147</v>
       </c>
       <c r="C18" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="74" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>148</v>
@@ -5389,7 +5392,7 @@
         <v>149</v>
       </c>
       <c r="C20" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -5397,15 +5400,15 @@
         <v>150</v>
       </c>
       <c r="C21" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C22" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -5413,7 +5416,7 @@
         <v>151</v>
       </c>
       <c r="C23" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -5421,7 +5424,7 @@
         <v>152</v>
       </c>
       <c r="C24" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
@@ -5429,7 +5432,7 @@
         <v>153</v>
       </c>
       <c r="C25" s="42" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -5473,8 +5476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76841965-3DC3-4506-A9BF-4F5122DFDEF3}">
   <dimension ref="A1:M171"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="102" zoomScaleNormal="100" zoomScalePageLayoutView="102" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E2"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A47" zoomScale="102" zoomScaleNormal="100" zoomScalePageLayoutView="102" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -5504,7 +5507,7 @@
       <c r="D1" s="83"/>
       <c r="E1" s="83"/>
       <c r="F1" s="79" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G1" s="79"/>
       <c r="H1" s="79"/>
@@ -5522,7 +5525,7 @@
       <c r="D2" s="85"/>
       <c r="E2" s="85"/>
       <c r="F2" s="80" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G2" s="81"/>
       <c r="H2" s="81"/>
@@ -5558,7 +5561,7 @@
         <v>166</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J3" s="13" t="s">
         <v>167</v>
@@ -5695,7 +5698,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" s="15" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C12" s="26"/>
       <c r="D12" s="28"/>
@@ -5725,7 +5728,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B14" s="15" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C14" s="26"/>
       <c r="D14" s="28"/>
@@ -6658,7 +6661,7 @@
     </row>
     <row r="85" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B85" s="15" t="s">
-        <v>240</v>
+        <v>519</v>
       </c>
       <c r="C85" s="26"/>
       <c r="D85" s="28"/>
@@ -6673,7 +6676,7 @@
     </row>
     <row r="86" spans="2:12" ht="25.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B86" s="19" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="87" spans="2:12" x14ac:dyDescent="0.2">
@@ -6681,7 +6684,7 @@
     </row>
     <row r="88" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B88" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C88" s="26"/>
       <c r="D88" s="28"/>
@@ -6696,7 +6699,7 @@
     </row>
     <row r="89" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B89" s="15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C89" s="26"/>
       <c r="D89" s="28"/>
@@ -6711,7 +6714,7 @@
     </row>
     <row r="90" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B90" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C90" s="26"/>
       <c r="D90" s="28"/>
@@ -6726,7 +6729,7 @@
     </row>
     <row r="91" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B91" s="15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C91" s="26"/>
       <c r="D91" s="28"/>
@@ -6741,7 +6744,7 @@
     </row>
     <row r="92" spans="2:12" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B92" s="19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="93" spans="2:12" x14ac:dyDescent="0.2">
@@ -6749,7 +6752,7 @@
     </row>
     <row r="94" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B94" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C94" s="26"/>
       <c r="D94" s="28"/>
@@ -6764,7 +6767,7 @@
     </row>
     <row r="95" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B95" s="15" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C95" s="26"/>
       <c r="D95" s="28"/>
@@ -6779,7 +6782,7 @@
     </row>
     <row r="96" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B96" s="15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C96" s="26"/>
       <c r="D96" s="28"/>
@@ -6794,7 +6797,7 @@
     </row>
     <row r="97" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B97" s="15" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C97" s="26"/>
       <c r="D97" s="28"/>
@@ -6809,7 +6812,7 @@
     </row>
     <row r="98" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B98" s="15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C98" s="26"/>
       <c r="D98" s="28"/>
@@ -6824,7 +6827,7 @@
     </row>
     <row r="99" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B99" s="15" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C99" s="26"/>
       <c r="D99" s="28"/>
@@ -6839,7 +6842,7 @@
     </row>
     <row r="100" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B100" s="15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C100" s="26"/>
       <c r="D100" s="28"/>
@@ -6854,7 +6857,7 @@
     </row>
     <row r="101" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B101" s="15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C101" s="26"/>
       <c r="D101" s="28"/>
@@ -6869,7 +6872,7 @@
     </row>
     <row r="102" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B102" s="15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C102" s="26"/>
       <c r="D102" s="28"/>
@@ -6884,7 +6887,7 @@
     </row>
     <row r="103" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B103" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C103" s="26"/>
       <c r="D103" s="28"/>
@@ -6899,7 +6902,7 @@
     </row>
     <row r="104" spans="2:12" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B104" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="105" spans="2:12" x14ac:dyDescent="0.2">
@@ -6907,7 +6910,7 @@
     </row>
     <row r="106" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B106" s="17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C106" s="26"/>
       <c r="D106" s="28"/>
@@ -6922,7 +6925,7 @@
     </row>
     <row r="107" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B107" s="15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C107" s="26"/>
       <c r="D107" s="28"/>
@@ -6937,7 +6940,7 @@
     </row>
     <row r="108" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B108" s="15" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C108" s="26"/>
       <c r="D108" s="28"/>
@@ -6952,7 +6955,7 @@
     </row>
     <row r="109" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B109" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C109" s="26"/>
       <c r="D109" s="28"/>
@@ -6967,7 +6970,7 @@
     </row>
     <row r="110" spans="2:12" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B110" s="19" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="111" spans="2:12" x14ac:dyDescent="0.2">
@@ -6975,7 +6978,7 @@
     </row>
     <row r="112" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B112" s="17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C112" s="26"/>
       <c r="D112" s="28"/>
@@ -6990,7 +6993,7 @@
     </row>
     <row r="113" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B113" s="15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C113" s="26"/>
       <c r="D113" s="28"/>
@@ -7005,7 +7008,7 @@
     </row>
     <row r="114" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B114" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C114" s="26"/>
       <c r="D114" s="28"/>
@@ -7020,7 +7023,7 @@
     </row>
     <row r="115" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B115" s="15" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C115" s="26"/>
       <c r="D115" s="28"/>
@@ -7065,7 +7068,7 @@
     </row>
     <row r="118" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B118" s="15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C118" s="26"/>
       <c r="D118" s="28"/>
@@ -7080,7 +7083,7 @@
     </row>
     <row r="119" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B119" s="15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C119" s="26"/>
       <c r="D119" s="28"/>
@@ -7095,7 +7098,7 @@
     </row>
     <row r="120" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B120" s="19" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="121" spans="2:12" x14ac:dyDescent="0.2">
@@ -7103,7 +7106,7 @@
     </row>
     <row r="122" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B122" s="17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C122" s="26"/>
       <c r="D122" s="28"/>
@@ -7118,7 +7121,7 @@
     </row>
     <row r="123" spans="2:12" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B123" s="19" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="124" spans="2:12" x14ac:dyDescent="0.2">
@@ -7126,7 +7129,7 @@
     </row>
     <row r="125" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B125" s="17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C125" s="26"/>
       <c r="D125" s="28"/>
@@ -7141,7 +7144,7 @@
     </row>
     <row r="126" spans="2:12" ht="24.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B126" s="19" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="127" spans="2:12" x14ac:dyDescent="0.2">
@@ -7149,7 +7152,7 @@
     </row>
     <row r="128" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B128" s="17" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C128" s="26"/>
       <c r="D128" s="28"/>
@@ -7164,7 +7167,7 @@
     </row>
     <row r="129" spans="2:12" ht="30" x14ac:dyDescent="0.2">
       <c r="B129" s="23" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C129" s="26"/>
       <c r="D129" s="28"/>
@@ -7179,7 +7182,7 @@
     </row>
     <row r="130" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B130" s="15" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C130" s="26"/>
       <c r="D130" s="28"/>
@@ -7194,7 +7197,7 @@
     </row>
     <row r="131" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B131" s="15" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C131" s="26"/>
       <c r="D131" s="28"/>
@@ -7209,7 +7212,7 @@
     </row>
     <row r="132" spans="2:12" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B132" s="19" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="133" spans="2:12" x14ac:dyDescent="0.2">
@@ -7217,7 +7220,7 @@
     </row>
     <row r="134" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B134" s="17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C134" s="26"/>
       <c r="D134" s="28"/>
@@ -7232,7 +7235,7 @@
     </row>
     <row r="135" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B135" s="15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C135" s="26"/>
       <c r="D135" s="28"/>
@@ -7247,7 +7250,7 @@
     </row>
     <row r="136" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B136" s="15" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C136" s="26"/>
       <c r="D136" s="28"/>
@@ -7262,7 +7265,7 @@
     </row>
     <row r="137" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B137" s="15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C137" s="26"/>
       <c r="D137" s="28"/>
@@ -7277,7 +7280,7 @@
     </row>
     <row r="138" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B138" s="15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C138" s="26"/>
       <c r="D138" s="28"/>
@@ -7292,7 +7295,7 @@
     </row>
     <row r="139" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B139" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="140" spans="2:12" x14ac:dyDescent="0.2">
@@ -7300,7 +7303,7 @@
     </row>
     <row r="141" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B141" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C141" s="26"/>
       <c r="D141" s="28"/>
@@ -7315,7 +7318,7 @@
     </row>
     <row r="142" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B142" s="19" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="143" spans="2:12" x14ac:dyDescent="0.2">
@@ -7323,7 +7326,7 @@
     </row>
     <row r="144" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B144" s="17" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C144" s="26"/>
       <c r="D144" s="28"/>
@@ -7338,7 +7341,7 @@
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B145" s="15" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C145" s="26"/>
       <c r="D145" s="28"/>
@@ -7353,7 +7356,7 @@
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B146" s="15" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C146" s="26"/>
       <c r="D146" s="28"/>
@@ -7368,7 +7371,7 @@
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B147" s="15" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C147" s="26"/>
       <c r="D147" s="28"/>
@@ -7383,7 +7386,7 @@
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B148" s="15" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C148" s="26"/>
       <c r="D148" s="28"/>
@@ -7398,7 +7401,7 @@
     </row>
     <row r="149" spans="1:13" ht="22.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B149" s="19" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.2">
@@ -7406,7 +7409,7 @@
     </row>
     <row r="151" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="B151" s="24" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C151" s="26"/>
       <c r="D151" s="28"/>
@@ -7421,7 +7424,7 @@
     </row>
     <row r="152" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B152" s="19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.2">
@@ -7429,7 +7432,7 @@
     </row>
     <row r="154" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="B154" s="24" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C154" s="26"/>
       <c r="D154" s="28"/>
@@ -7444,7 +7447,7 @@
     </row>
     <row r="155" spans="1:13" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B155" s="19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.2">
@@ -7467,7 +7470,7 @@
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B158" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F158" s="15" cm="1">
         <f t="array" ref="F158">SUM(SUMPRODUCT(($C$4:$C$154="x")*(F4:F154="x")*1),(SUMPRODUCT(($D$4:$D$154="x")*(F4:F154="x")*1)))</f>
@@ -7500,7 +7503,7 @@
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B159" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C159" s="6"/>
       <c r="D159" s="6"/>
@@ -7536,7 +7539,7 @@
     </row>
     <row r="160" spans="1:13" ht="60" x14ac:dyDescent="0.2">
       <c r="B160" s="18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C160" s="7">
         <f>COUNTIF(C4:C154,"x")</f>
@@ -7560,7 +7563,7 @@
         <v>166</v>
       </c>
       <c r="I160" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J160" s="13" t="s">
         <v>167</v>
@@ -7572,15 +7575,15 @@
         <v>169</v>
       </c>
       <c r="M160" s="57" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A162" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="B162" s="86" t="s">
         <v>300</v>
-      </c>
-      <c r="B162" s="86" t="s">
-        <v>301</v>
       </c>
       <c r="C162" s="86"/>
       <c r="D162" s="86"/>
@@ -7601,7 +7604,7 @@
       <c r="D163" s="85"/>
       <c r="E163" s="85"/>
       <c r="F163" s="87" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G163" s="79"/>
       <c r="H163" s="79"/>
@@ -7613,7 +7616,7 @@
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B164" s="20" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C164" s="85"/>
       <c r="D164" s="85"/>
@@ -7629,7 +7632,7 @@
     </row>
     <row r="165" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="B165" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C165" s="85"/>
       <c r="D165" s="85"/>
@@ -7645,7 +7648,7 @@
     </row>
     <row r="166" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="B166" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C166" s="85"/>
       <c r="D166" s="85"/>
@@ -7661,10 +7664,10 @@
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B167" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C167" s="82" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D167" s="82"/>
       <c r="E167" s="82"/>
@@ -7679,7 +7682,7 @@
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B168" s="20" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C168" s="85"/>
       <c r="D168" s="85"/>
@@ -7695,10 +7698,10 @@
     </row>
     <row r="169" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="B169" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C169" s="82" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D169" s="82"/>
       <c r="E169" s="82"/>
@@ -7713,10 +7716,10 @@
     </row>
     <row r="170" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="B170" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C170" s="82" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D170" s="82"/>
       <c r="E170" s="82"/>
@@ -7731,7 +7734,7 @@
     </row>
     <row r="171" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="B171" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F171" s="85"/>
       <c r="G171" s="85"/>
@@ -7804,31 +7807,31 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
+        <v>311</v>
+      </c>
+      <c r="B1" s="31" t="s">
         <v>312</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>313</v>
       </c>
       <c r="C1" s="31" t="s">
         <v>114</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="88" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C2" s="88"/>
       <c r="D2" s="88"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
+        <v>314</v>
+      </c>
+      <c r="B3" s="37" t="s">
         <v>315</v>
-      </c>
-      <c r="B3" s="37" t="s">
-        <v>316</v>
       </c>
       <c r="C3" s="38"/>
       <c r="D3" s="33" t="s">
@@ -7837,22 +7840,22 @@
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="B4" s="39" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D4" s="34"/>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="B5" s="39" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D5" s="34"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
+        <v>316</v>
+      </c>
+      <c r="B6" s="37" t="s">
         <v>317</v>
-      </c>
-      <c r="B6" s="37" t="s">
-        <v>318</v>
       </c>
       <c r="C6" s="37"/>
       <c r="D6" s="33" t="s">
@@ -7861,133 +7864,133 @@
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="B7" s="39" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D7" s="34"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="35" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D8" s="34"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D9" s="34"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D10" s="34"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="35" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D11" s="34"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="35" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D12" s="34"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D13" s="34"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D14" s="34"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D15" s="34"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D16" s="34"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D17" s="34"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D18" s="34"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="35" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D19" s="34"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D20" s="34"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D21" s="34"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D22" s="34"/>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="B23" s="39" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D23" s="34"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D24" s="34"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D25" s="34"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D26" s="34"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D27" s="34"/>
     </row>
     <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B28" s="40" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D28" s="34"/>
     </row>
@@ -7996,10 +7999,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="36" t="s">
+        <v>341</v>
+      </c>
+      <c r="B30" s="37" t="s">
         <v>342</v>
-      </c>
-      <c r="B30" s="37" t="s">
-        <v>343</v>
       </c>
       <c r="C30" s="37"/>
       <c r="D30" s="33" t="s">
@@ -8008,164 +8011,164 @@
     </row>
     <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B31" s="40" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D31" s="34"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" s="35" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D32" s="34"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D33" s="34"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D34" s="34"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D35" s="34"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D36" s="34"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D37" s="34"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="36" t="s">
+        <v>350</v>
+      </c>
+      <c r="B38" s="37" t="s">
         <v>351</v>
-      </c>
-      <c r="B38" s="37" t="s">
-        <v>352</v>
       </c>
       <c r="C38" s="37"/>
       <c r="D38" s="37"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="35" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B46" s="35" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B47" s="35" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B49" s="35" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B50" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B51" s="35" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B52" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B53" s="35" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B54" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B55" s="35" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B56" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B57" s="35" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B58" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B59" s="35" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B60" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -8203,16 +8206,16 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="58" t="s">
+        <v>365</v>
+      </c>
+      <c r="B1" s="59" t="s">
         <v>366</v>
-      </c>
-      <c r="B1" s="59" t="s">
-        <v>367</v>
       </c>
       <c r="C1" s="59"/>
     </row>
     <row r="2" spans="1:3" ht="41.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="84" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C2" s="84"/>
     </row>
@@ -8220,15 +8223,15 @@
       <c r="A3" s="46"/>
       <c r="B3" s="46"/>
       <c r="C3" s="46" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="B4" s="45" t="s">
         <v>374</v>
-      </c>
-      <c r="B4" s="45" t="s">
-        <v>375</v>
       </c>
       <c r="C4" s="45"/>
     </row>
@@ -8240,40 +8243,40 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6" s="44" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C6" s="60"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="44" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C7" s="60"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B8" s="44" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C8" s="60"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" s="44" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C9" s="60"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10" s="44" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C10" s="60"/>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="B11" s="61" t="s">
         <v>376</v>
-      </c>
-      <c r="B11" s="61" t="s">
-        <v>377</v>
       </c>
       <c r="C11" s="45"/>
     </row>
@@ -8285,193 +8288,193 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B13" s="44" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C13" s="60"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B14" s="44" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C14" s="60"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B15" s="44" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C15" s="60"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B16" s="44" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C16" s="60"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="B17" s="45" t="s">
         <v>378</v>
-      </c>
-      <c r="B17" s="45" t="s">
-        <v>379</v>
       </c>
       <c r="C17" s="45"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B18" s="44" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C18" s="60"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B19" s="44" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C19" s="60"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B20" s="44" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C20" s="60"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B21" s="44" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C21" s="60"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="B22" s="45" t="s">
         <v>383</v>
-      </c>
-      <c r="B22" s="45" t="s">
-        <v>384</v>
       </c>
       <c r="C22" s="45"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B23" s="44" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C23" s="60"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B24" s="44" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C24" s="60"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B25" s="44" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C25" s="60"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B26" s="44" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C26" s="60"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B27" s="44" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C27" s="60"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B28" s="44" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C28" s="60"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B29" s="44" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C29" s="60"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B30" s="44" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C30" s="60"/>
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
+        <v>391</v>
+      </c>
+      <c r="B31" s="61" t="s">
         <v>392</v>
-      </c>
-      <c r="B31" s="61" t="s">
-        <v>393</v>
       </c>
       <c r="C31" s="45"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B32" s="44" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C32" s="60"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B33" s="44" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C33" s="60"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B34" s="44" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C34" s="60"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B35" s="45" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C35" s="45"/>
     </row>
     <row r="36" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="B36" s="43" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C36" s="60"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B37" s="45" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C37" s="45"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B38" s="44" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C38" s="60"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B39" s="44" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C39" s="60"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B40" s="45" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C40" s="45"/>
     </row>
     <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="B41" s="43" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C41" s="60"/>
     </row>

</xml_diff>